<commit_message>
feat: Add project parameters and Saint-Gobain product database files.
</commit_message>
<xml_diff>
--- a/data/parameters_config/project_parameters.xlsx
+++ b/data/parameters_config/project_parameters.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="96">
   <si>
     <t>Category</t>
   </si>
@@ -308,18 +308,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -332,41 +324,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF555555"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1F4E78"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDEBF7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -396,22 +360,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,12 +664,6 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="60.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -734,758 +680,758 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3">
         <v>2500</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5">
         <v>10</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6">
         <v>30</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7">
         <v>1400</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8">
         <v>0.05</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9">
         <v>0.77</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10">
         <v>1.29</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11">
         <v>4.683</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12">
         <v>4</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13">
         <v>0.57</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14">
         <v>0.17</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15">
         <v>0.14</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16">
         <v>0.27</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17">
         <v>0.3</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18">
         <v>0.39</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19">
         <v>24000</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20">
         <v>0.05</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22">
+        <v>0.15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23">
+        <v>0.15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25">
+        <v>1.5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31">
+        <v>0.01</v>
+      </c>
+      <c r="D31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32">
+        <v>0.02</v>
+      </c>
+      <c r="D32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33">
+        <v>0.95</v>
+      </c>
+      <c r="D33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34">
+        <v>0.9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35">
+        <v>0.1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36">
+        <v>0.2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37">
+        <v>0.2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38">
+        <v>0.8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39">
+        <v>0.1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40">
+        <v>0.1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41">
+        <v>30</v>
+      </c>
+      <c r="D41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42">
         <v>0</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="4">
-        <v>0</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="4">
-        <v>1</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="4">
-        <v>1</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="4">
-        <v>1</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="4">
-        <v>3</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="4">
-        <v>1</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="4">
-        <v>2</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="3" t="s">
+      <c r="D42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43">
+        <v>100</v>
+      </c>
+      <c r="D43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44">
+        <v>150</v>
+      </c>
+      <c r="D44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45">
+        <v>80</v>
+      </c>
+      <c r="D45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47">
+        <v>1.6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48">
         <v>50</v>
       </c>
-      <c r="C39" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" s="4">
-        <v>30</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42" s="4">
-        <v>0</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="4">
+      <c r="D48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49">
         <v>100</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" s="4">
-        <v>150</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="4">
-        <v>80</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="2" t="s">
+      <c r="D49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="2" t="s">
+      <c r="B50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50">
+        <v>0.015</v>
+      </c>
+      <c r="D50" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
         <v>12</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48" s="4">
-        <v>50</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="2" t="s">
+      <c r="B51" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51">
+        <v>0.062</v>
+      </c>
+      <c r="D51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C49" s="4">
-        <v>100</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="2" t="s">
+      <c r="B52" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52">
+        <v>500</v>
+      </c>
+      <c r="D52" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C50" s="4">
-        <v>0.015</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="2" t="s">
+      <c r="B53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C51" s="4">
-        <v>0.062</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="2" t="s">
+      <c r="B54" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D54" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
         <v>12</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" s="4">
-        <v>500</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" t="s">
         <v>66</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C55">
         <v>24</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>